<commit_message>
week 4 first draft - not yet checked for mistakes
</commit_message>
<xml_diff>
--- a/src/activities/data/paralympics_all_raw.xlsx
+++ b/src/activities/data/paralympics_all_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/COMP0035-tutorials-2025/src/activities/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD1159D-564B-A646-B168-9F70EFB703C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E298C3-1EF2-0C4B-96E1-5B20F1A5FF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17200" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
   </bookViews>
@@ -3440,7 +3440,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>